<commit_message>
Add outlier analysis and update player profiles
</commit_message>
<xml_diff>
--- a/Documentation/Termplate burndown.xlsx
+++ b/Documentation/Termplate burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Batsman_bowler_matchup\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4EEFB9-3623-47AC-99FA-96E2A77F4AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67F0B5C-2CB8-48B6-9C48-20E2DF56DDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sprint_02 BurnDown Chart" sheetId="6" r:id="rId4"/>
     <sheet name="Sprint_03 BurnDown Chart" sheetId="7" r:id="rId5"/>
     <sheet name="Sprint_04 BurnDown Chart" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="69">
   <si>
     <t>Backlog ID</t>
   </si>
@@ -232,10 +233,22 @@
     <t>Frontend for Predictions</t>
   </si>
   <si>
-    <t>Backend for Dynamic Dropdowns</t>
+    <t>Profile Page</t>
   </si>
   <si>
-    <t>Backend for Predictions</t>
+    <t xml:space="preserve">Player Comparison </t>
+  </si>
+  <si>
+    <t>Analysis Page</t>
+  </si>
+  <si>
+    <t>SPRINT 5 BURNDOWN CHART</t>
+  </si>
+  <si>
+    <t>Project Testing</t>
+  </si>
+  <si>
+    <t>Documentaion</t>
   </si>
 </sst>
 </file>
@@ -1652,7 +1665,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint_03 BurnDown Chart'!$B$14</c:f>
+              <c:f>'Sprint_03 BurnDown Chart'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1731,57 +1744,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint_03 BurnDown Chart'!$C$14:$T$14</c:f>
+              <c:f>'Sprint_03 BurnDown Chart'!$C$12:$T$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1801,7 +1814,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint_03 BurnDown Chart'!$B$15</c:f>
+              <c:f>'Sprint_03 BurnDown Chart'!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1880,57 +1893,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint_03 BurnDown Chart'!$C$15:$T$15</c:f>
+              <c:f>'Sprint_03 BurnDown Chart'!$C$13:$T$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -2754,6 +2767,552 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>SPRINT 5 BURNDOWN CHART</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$5:$M$5</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BE5-45D5-A6A8-A301660DA72E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$5:$M$5</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$9:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6BE5-45D5-A6A8-A301660DA72E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1731720016"/>
+        <c:axId val="1731720496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1731720016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1731720496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1731720496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1731720016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2914,6 +3473,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4463,6 +5062,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5066,13 +6181,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>439917</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>8373</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>150725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5122,6 +6237,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3D0E570-CC35-D80C-110B-D3A128E5905A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>198783</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>53009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>503583</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>13252</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067D2A77-AD29-B5B2-509E-8F3239089416}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5764,7 +6920,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
       <c r="C22" s="9">
         <v>3004</v>
@@ -6060,8 +7216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342E0490-9415-4A7F-A774-0D7581BC698E}">
   <dimension ref="B2:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6440,7 +7596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F786CA-624D-46B6-B96B-C84F169FDEF2}">
   <dimension ref="B2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
@@ -6788,10 +7944,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F73131-84EF-4740-84E0-1C41110E54B6}">
-  <dimension ref="B2:T15"/>
+  <dimension ref="B2:T13"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6997,16 +8153,16 @@
         <v>42</v>
       </c>
       <c r="D7" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="5">
-        <v>2</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="5">
-        <v>2</v>
-      </c>
-      <c r="H7" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -7028,21 +8184,19 @@
         <v>43</v>
       </c>
       <c r="D8" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5">
-        <v>2</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1</v>
-      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -7053,28 +8207,28 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="9" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
-        <v>3004</v>
+        <v>3006</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5">
-        <v>3</v>
-      </c>
-      <c r="L9" s="5">
         <v>1</v>
       </c>
+      <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -7086,13 +8240,13 @@
     </row>
     <row r="10" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
-        <v>3005</v>
+        <v>3007</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D10" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -7103,7 +8257,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10" s="5">
         <v>1</v>
@@ -7117,251 +8271,187 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>3006</v>
+        <v>3008</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D11" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5">
-        <v>1</v>
-      </c>
+      <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5">
-        <v>1</v>
-      </c>
+      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5">
         <v>1</v>
       </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="P11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>1</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1</v>
+      </c>
+      <c r="S11" s="5">
+        <v>1</v>
+      </c>
       <c r="T11" s="5"/>
     </row>
-    <row r="12" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <v>3007</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>46</v>
-      </c>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="24"/>
       <c r="D12" s="5">
+        <f>SUM(D5:D11)</f>
+        <v>16</v>
+      </c>
+      <c r="E12" s="5">
+        <f>D12-SUM(E5:E11)</f>
+        <v>15</v>
+      </c>
+      <c r="F12" s="5">
+        <f>E12-SUM(F5:F11)</f>
+        <v>14</v>
+      </c>
+      <c r="G12" s="5">
+        <f>F12-SUM(G5:G11)</f>
+        <v>13</v>
+      </c>
+      <c r="H12" s="5">
+        <f>G12-SUM(H5:H11)</f>
+        <v>11</v>
+      </c>
+      <c r="I12" s="5">
+        <f>H12-SUM(I5:I11)</f>
+        <v>11</v>
+      </c>
+      <c r="J12" s="5">
+        <f>I12-SUM(J5:J11)</f>
+        <v>10</v>
+      </c>
+      <c r="K12" s="5">
+        <f>J12-SUM(K5:K11)</f>
+        <v>8</v>
+      </c>
+      <c r="L12" s="5">
+        <f>K12-SUM(L5:L11)</f>
+        <v>8</v>
+      </c>
+      <c r="M12" s="5">
+        <f>L12-SUM(M5:M11)</f>
+        <v>7</v>
+      </c>
+      <c r="N12" s="5">
+        <f>M12-SUM(N5:N11)</f>
+        <v>6</v>
+      </c>
+      <c r="O12" s="5">
+        <f>N12-SUM(O5:O11)</f>
+        <v>4</v>
+      </c>
+      <c r="P12" s="5">
+        <f>O12-SUM(P5:P11)</f>
+        <v>3</v>
+      </c>
+      <c r="Q12" s="5">
+        <f>P12-SUM(Q5:Q11)</f>
         <v>2</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5">
+      <c r="R12" s="5">
+        <f>Q12-SUM(R5:R11)</f>
         <v>1</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="S12" s="5">
+        <f>R12-SUM(S5:S11)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="5">
+        <f>S12-SUM(T5:T11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="5">
+        <v>16</v>
+      </c>
+      <c r="E13" s="5">
+        <f>$D$13-($D$13/16*1)</f>
+        <v>15</v>
+      </c>
+      <c r="F13" s="5">
+        <f>$D$13-($D$13/16*2)</f>
+        <v>14</v>
+      </c>
+      <c r="G13" s="5">
+        <f>$D$13-($D$13/16*3)</f>
+        <v>13</v>
+      </c>
+      <c r="H13" s="5">
+        <f>$D$13-($D$13/16*4)</f>
+        <v>12</v>
+      </c>
+      <c r="I13" s="5">
+        <f>$D$13-($D$13/16*5)</f>
+        <v>11</v>
+      </c>
+      <c r="J13" s="5">
+        <f>$D$13-($D$13/16*6)</f>
+        <v>10</v>
+      </c>
+      <c r="K13" s="5">
+        <f>$D$13-($D$13/16*7)</f>
+        <v>9</v>
+      </c>
+      <c r="L13" s="5">
+        <f>$D$13-($D$13/16*8)</f>
+        <v>8</v>
+      </c>
+      <c r="M13" s="5">
+        <f>$D$13-($D$13/16*9)</f>
+        <v>7</v>
+      </c>
+      <c r="N13" s="5">
+        <f>$D$13-($D$13/16*10)</f>
+        <v>6</v>
+      </c>
+      <c r="O13" s="5">
+        <f>$D$13-($D$13/16*11)</f>
+        <v>5</v>
+      </c>
+      <c r="P13" s="5">
+        <f>$D$13-($D$13/16*12)</f>
+        <v>4</v>
+      </c>
+      <c r="Q13" s="5">
+        <f>$D$13-($D$13/16*13)</f>
+        <v>3</v>
+      </c>
+      <c r="R13" s="5">
+        <f>$D$13-($D$13/16*14)</f>
+        <v>2</v>
+      </c>
+      <c r="S13" s="5">
+        <f>$D$13-($D$13/16*15)</f>
         <v>1</v>
       </c>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <v>3008</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="5">
-        <v>8</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5">
-        <v>1</v>
-      </c>
-      <c r="R13" s="5">
-        <v>3</v>
-      </c>
-      <c r="S13" s="5">
-        <v>3</v>
-      </c>
       <c r="T13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="5">
-        <f>SUM(D5:D13)</f>
-        <v>32</v>
-      </c>
-      <c r="E14" s="5">
-        <f>D14-SUM(E5:E13)</f>
-        <v>31</v>
-      </c>
-      <c r="F14" s="5">
-        <f>E14-SUM(F5:F13)</f>
-        <v>28</v>
-      </c>
-      <c r="G14" s="5">
-        <f>F14-SUM(G5:G13)</f>
-        <v>26</v>
-      </c>
-      <c r="H14" s="5">
-        <f>G14-SUM(H5:H13)</f>
-        <v>23</v>
-      </c>
-      <c r="I14" s="5">
-        <f>H14-SUM(I5:I13)</f>
-        <v>22</v>
-      </c>
-      <c r="J14" s="5">
-        <f>I14-SUM(J5:J13)</f>
-        <v>21</v>
-      </c>
-      <c r="K14" s="5">
-        <f>J14-SUM(K5:K13)</f>
-        <v>17</v>
-      </c>
-      <c r="L14" s="5">
-        <f>K14-SUM(L5:L13)</f>
-        <v>16</v>
-      </c>
-      <c r="M14" s="5">
-        <f>L14-SUM(M5:M13)</f>
-        <v>13</v>
-      </c>
-      <c r="N14" s="5">
-        <f>M14-SUM(N5:N13)</f>
-        <v>12</v>
-      </c>
-      <c r="O14" s="5">
-        <f>N14-SUM(O5:O13)</f>
-        <v>10</v>
-      </c>
-      <c r="P14" s="5">
-        <f>O14-SUM(P5:P13)</f>
-        <v>9</v>
-      </c>
-      <c r="Q14" s="5">
-        <f>P14-SUM(Q5:Q13)</f>
-        <v>7</v>
-      </c>
-      <c r="R14" s="5">
-        <f>Q14-SUM(R5:R13)</f>
-        <v>4</v>
-      </c>
-      <c r="S14" s="5">
-        <f>R14-SUM(S5:S13)</f>
-        <v>1</v>
-      </c>
-      <c r="T14" s="5">
-        <f>S14-SUM(T5:T13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="5">
-        <v>32</v>
-      </c>
-      <c r="E15" s="5">
-        <f>$D$15-($D$15/16*1)</f>
-        <v>30</v>
-      </c>
-      <c r="F15" s="5">
-        <f>$D$15-($D$15/16*2)</f>
-        <v>28</v>
-      </c>
-      <c r="G15" s="5">
-        <f>$D$15-($D$15/16*3)</f>
-        <v>26</v>
-      </c>
-      <c r="H15" s="5">
-        <f>$D$15-($D$15/16*4)</f>
-        <v>24</v>
-      </c>
-      <c r="I15" s="5">
-        <f>$D$15-($D$15/16*5)</f>
-        <v>22</v>
-      </c>
-      <c r="J15" s="5">
-        <f>$D$15-($D$15/16*6)</f>
-        <v>20</v>
-      </c>
-      <c r="K15" s="5">
-        <f>$D$15-($D$15/16*7)</f>
-        <v>18</v>
-      </c>
-      <c r="L15" s="5">
-        <f>$D$15-($D$15/16*8)</f>
-        <v>16</v>
-      </c>
-      <c r="M15" s="5">
-        <f>$D$15-($D$15/16*9)</f>
-        <v>14</v>
-      </c>
-      <c r="N15" s="5">
-        <f>$D$15-($D$15/16*10)</f>
-        <v>12</v>
-      </c>
-      <c r="O15" s="5">
-        <f>$D$15-($D$15/16*11)</f>
-        <v>10</v>
-      </c>
-      <c r="P15" s="5">
-        <f>$D$15-($D$15/16*12)</f>
-        <v>8</v>
-      </c>
-      <c r="Q15" s="5">
-        <f>$D$15-($D$15/16*13)</f>
-        <v>6</v>
-      </c>
-      <c r="R15" s="5">
-        <f>$D$15-($D$15/16*14)</f>
-        <v>4</v>
-      </c>
-      <c r="S15" s="5">
-        <f>$D$15-($D$15/16*15)</f>
-        <v>2</v>
-      </c>
-      <c r="T15" s="5">
-        <f>$D$15-($D$15/16*16)</f>
+        <f>$D$13-($D$13/16*16)</f>
         <v>0</v>
       </c>
     </row>
@@ -7369,8 +8459,8 @@
   <mergeCells count="6">
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B2:T2"/>
     <mergeCell ref="B3:T3"/>
   </mergeCells>
@@ -7384,8 +8474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AF9155-10A4-43E3-9B0E-4BED5400B97D}">
   <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7519,7 +8609,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>4002</v>
       </c>
@@ -7541,12 +8631,12 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>4003</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5">
         <v>2</v>
@@ -7565,12 +8655,12 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>4004</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5">
         <v>2</v>
@@ -7764,4 +8854,282 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A1524D-E823-4B5F-B997-62B5BB90B27A}">
+  <dimension ref="B2:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6">
+        <v>45901</v>
+      </c>
+      <c r="F4" s="6">
+        <v>46266</v>
+      </c>
+      <c r="G4" s="6">
+        <v>46631</v>
+      </c>
+      <c r="H4" s="6">
+        <v>46997</v>
+      </c>
+      <c r="I4" s="6">
+        <v>47362</v>
+      </c>
+      <c r="J4" s="6">
+        <v>47727</v>
+      </c>
+      <c r="K4" s="6">
+        <v>37165</v>
+      </c>
+      <c r="L4" s="6">
+        <v>37530</v>
+      </c>
+      <c r="M4" s="6">
+        <v>37895</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>4001</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>4002</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="5">
+        <f>SUM(D5:D7)</f>
+        <v>9</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8-SUM(E5:E7)</f>
+        <v>8</v>
+      </c>
+      <c r="F8" s="5">
+        <f>E8-SUM(F5:F7)</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <f>F8-SUM(G5:G7)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="5">
+        <f>G8-SUM(H5:H7)</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="5">
+        <f>H8-SUM(I5:I7)</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="5">
+        <f>I8-SUM(J5:J7)</f>
+        <v>2</v>
+      </c>
+      <c r="K8" s="5">
+        <f>J8-SUM(K5:K7)</f>
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <f>K8-SUM(L5:L7)</f>
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <f>L8-SUM(M5:M7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="5">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5">
+        <f>$D$9-($D$9/9*1)</f>
+        <v>8</v>
+      </c>
+      <c r="F9" s="5">
+        <f>$D$9-($D$9/9*2)</f>
+        <v>7</v>
+      </c>
+      <c r="G9" s="5">
+        <f>$D$9-($D$9/9*3)</f>
+        <v>6</v>
+      </c>
+      <c r="H9" s="5">
+        <f>$D$9-($D$9/9*4)</f>
+        <v>5</v>
+      </c>
+      <c r="I9" s="5">
+        <f>$D$9-($D$9/9*5)</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="5">
+        <f>$D$9-($D$9/9*6)</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="5">
+        <f>$D$9-($D$9/9*7)</f>
+        <v>2</v>
+      </c>
+      <c r="L9" s="5">
+        <f>$D$9-($D$9/9*8)</f>
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <f>$D$9-($D$9/9*9)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor: Project cleanup, remove unused files and old models
</commit_message>
<xml_diff>
--- a/Documentation/Termplate burndown.xlsx
+++ b/Documentation/Termplate burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Batsman_bowler_matchup\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67F0B5C-2CB8-48B6-9C48-20E2DF56DDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F5190E-DEF0-40BD-8649-1B5F96037D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,7 +248,7 @@
     <t>Project Testing</t>
   </si>
   <si>
-    <t>Documentaion</t>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -6721,7 +6721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="122" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="122" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:B39"/>
     </sheetView>
   </sheetViews>
@@ -7217,7 +7217,7 @@
   <dimension ref="B2:N14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="B6" sqref="B6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7597,7 +7597,7 @@
   <dimension ref="B2:N22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="B6" sqref="B6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7946,8 +7946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F73131-84EF-4740-84E0-1C41110E54B6}">
   <dimension ref="B2:T13"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView zoomScale="77" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8209,7 +8209,7 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>45</v>
@@ -8240,7 +8240,7 @@
     </row>
     <row r="10" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>46</v>
@@ -8273,7 +8273,7 @@
     </row>
     <row r="11" spans="2:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>47</v>
@@ -8318,67 +8318,67 @@
         <v>16</v>
       </c>
       <c r="E12" s="5">
-        <f>D12-SUM(E5:E11)</f>
+        <f t="shared" ref="E12:T12" si="0">D12-SUM(E5:E11)</f>
         <v>15</v>
       </c>
       <c r="F12" s="5">
-        <f>E12-SUM(F5:F11)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G12" s="5">
-        <f>F12-SUM(G5:G11)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H12" s="5">
-        <f>G12-SUM(H5:H11)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I12" s="5">
-        <f>H12-SUM(I5:I11)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="J12" s="5">
-        <f>I12-SUM(J5:J11)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K12" s="5">
-        <f>J12-SUM(K5:K11)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L12" s="5">
-        <f>K12-SUM(L5:L11)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="M12" s="5">
-        <f>L12-SUM(M5:M11)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="N12" s="5">
-        <f>M12-SUM(N5:N11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="O12" s="5">
-        <f>N12-SUM(O5:O11)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P12" s="5">
-        <f>O12-SUM(P5:P11)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Q12" s="5">
-        <f>P12-SUM(Q5:Q11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R12" s="5">
-        <f>Q12-SUM(R5:R11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="S12" s="5">
-        <f>R12-SUM(S5:S11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T12" s="5">
-        <f>S12-SUM(T5:T11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8475,7 +8475,7 @@
   <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8860,8 +8860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A1524D-E823-4B5F-B997-62B5BB90B27A}">
   <dimension ref="B2:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8971,9 +8971,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
-        <v>4001</v>
+        <v>5001</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>67</v>
@@ -8995,9 +8995,9 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
-        <v>4002</v>
+        <v>5002</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>68</v>
@@ -9039,39 +9039,39 @@
         <v>9</v>
       </c>
       <c r="E8" s="5">
-        <f>D8-SUM(E5:E7)</f>
+        <f t="shared" ref="E8:M8" si="0">D8-SUM(E5:E7)</f>
         <v>8</v>
       </c>
       <c r="F8" s="5">
-        <f>E8-SUM(F5:F7)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G8" s="5">
-        <f>F8-SUM(G5:G7)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H8" s="5">
-        <f>G8-SUM(H5:H7)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I8" s="5">
-        <f>H8-SUM(I5:I7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J8" s="5">
-        <f>I8-SUM(J5:J7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K8" s="5">
-        <f>J8-SUM(K5:K7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8" s="5">
-        <f>K8-SUM(L5:L7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M8" s="5">
-        <f>L8-SUM(M5:M7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9122,12 +9122,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>